<commit_message>
Product backlog Janeth cambios
</commit_message>
<xml_diff>
--- a/Gestión de Proyecto/Product Backlog.xlsx
+++ b/Gestión de Proyecto/Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d34079dce998fb61/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\repositorio nat\ProyIntComDat25B_Twisted\Gestión de Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4521E4E2-7C96-4561-8FD8-9298865DC70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87F8AC6-7AEB-46E7-A286-0C4A598AA0E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="71">
   <si>
     <t>Columna</t>
   </si>
@@ -193,6 +193,72 @@
   </si>
   <si>
     <t>Es una tarea de comunicación, no de desarrollo del producto principal, pero es clave para su adopción.</t>
+  </si>
+  <si>
+    <t>HU-006</t>
+  </si>
+  <si>
+    <t>Como asesor estudiantil, quiero recibir una capacitación formal sobre el proceso de baja de materias, para poder informar verbalmente y con precisión a los alumnos.</t>
+  </si>
+  <si>
+    <t>Capacitación a Asesores</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Asegurar que el 70% de los asesores estén capacitados antes del lanzamiento.</t>
+  </si>
+  <si>
+    <t>HU-007</t>
+  </si>
+  <si>
+    <t>Como coordinador, quiero medir el porcentaje de estudiantes alcanzados por la campaña, para evaluar el impacto y realizar mejoras.</t>
+  </si>
+  <si>
+    <t>Métricas de Alcance</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Se debe contactar al menos al 90% de los estudiantes.</t>
+  </si>
+  <si>
+    <t>HU-008</t>
+  </si>
+  <si>
+    <t>Como responsable de comunicación, quiero verificar que la difusión cumpla con el reglamento universitario, para prevenir problemas de autorización.</t>
+  </si>
+  <si>
+    <t>Cumplimiento Normativo</t>
+  </si>
+  <si>
+    <t>Requiere validación formal por parte de la coordinación académica.</t>
+  </si>
+  <si>
+    <t>HU-009</t>
+  </si>
+  <si>
+    <t>Como diseñador, quiero crear material gráfico claro y atractivo (infografías, carteles), para facilitar la comprensión de fechas y procesos.</t>
+  </si>
+  <si>
+    <t>Material Gráfico</t>
+  </si>
+  <si>
+    <t>Deben aprobarse al menos 3 materiales gráficos.</t>
+  </si>
+  <si>
+    <t>HU-010</t>
+  </si>
+  <si>
+    <t>Como estudiante, quiero recibir un correo masivo con la información clave, para asegurarme de no perder las fechas importantes.</t>
+  </si>
+  <si>
+    <t>Correo Masivo</t>
+  </si>
+  <si>
+    <t>Envío a más del 90% de las cuentas institucionales.</t>
   </si>
 </sst>
 </file>
@@ -292,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -316,6 +382,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I18"/>
+  <dimension ref="B1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +708,7 @@
     <col min="5" max="5" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="84.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.140625" style="2" customWidth="1"/>
     <col min="11" max="16384" width="11.42578125" style="2"/>
@@ -805,79 +877,139 @@
       <c r="H9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="8" t="s">
+    <row r="10" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="7">
+        <v>5</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="7">
         <v>8</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="G11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="7">
+        <v>5</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="7">
+        <v>5</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="7">
         <v>8</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
+      <c r="G14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -934,6 +1066,110 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1048,14 +1284,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2622ba91-40fd-4640-b50c-92dc66e1fc44" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100346C637EA589F24D935192A732302EFF" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="83685da82484c26c18c41bb7d0d9a72e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2622ba91-40fd-4640-b50c-92dc66e1fc44" xmlns:ns4="749d5ae2-5db7-4e69-a7a3-6fccc2fcb882" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e614e9a4d0773a0fef6081f14e4182f" ns3:_="" ns4:_="">
     <xsd:import namespace="2622ba91-40fd-4640-b50c-92dc66e1fc44"/>
@@ -1282,6 +1510,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2622ba91-40fd-4640-b50c-92dc66e1fc44" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1292,23 +1528,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33A64BD6-8F16-4544-8B5D-AA544397FAEB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2622ba91-40fd-4640-b50c-92dc66e1fc44"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="749d5ae2-5db7-4e69-a7a3-6fccc2fcb882"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C969ACCE-2352-4E8C-A152-3EC477593924}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1327,6 +1546,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33A64BD6-8F16-4544-8B5D-AA544397FAEB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2622ba91-40fd-4640-b50c-92dc66e1fc44"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="749d5ae2-5db7-4e69-a7a3-6fccc2fcb882"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DA4B32A-075A-41C6-B17C-09D553423F42}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Brayan Cruz Cambios en Backlog
</commit_message>
<xml_diff>
--- a/Gestión de Proyecto/Product Backlog.xlsx
+++ b/Gestión de Proyecto/Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\repositorio jonathan\ProyIntComDat25B_Twisted\Gestión de Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braya\OneDrive\Documentos\2025-B\Parcial1\Proyecto integral de comunicaciones(Hazem)\Parcial1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7F8765-4C17-4A69-A240-54063088F782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F59313-3780-4C04-8E55-32654B1908AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="109">
   <si>
     <t>Columna</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Enunciado de la Historia</t>
   </si>
   <si>
-    <t>XX-XXXX-XXXX</t>
-  </si>
-  <si>
     <t>Desarrollo ágil: Pila de Producto (Product Backlog)</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
   </si>
   <si>
     <t>Elaborado por: pmoinformatica.com</t>
-  </si>
-  <si>
-    <t>Como un [Rol], necesito [descripción de la funcionalidad], con la finalidad de [Razón o Resultado]</t>
   </si>
   <si>
     <t>Estado</t>
@@ -320,12 +314,72 @@
   <si>
     <t>Colocar en al menos 5 puntos estratégicos de la universidad.</t>
   </si>
+  <si>
+    <t>Evalución de resultados</t>
+  </si>
+  <si>
+    <t>Hacer encuesta a 50 alumnos.</t>
+  </si>
+  <si>
+    <t>HU-016</t>
+  </si>
+  <si>
+    <t>HU-017</t>
+  </si>
+  <si>
+    <t>Rendimiento de la campaña</t>
+  </si>
+  <si>
+    <t>Con ayuda de las ecuestas se hace un analisis.</t>
+  </si>
+  <si>
+    <t>HU-018</t>
+  </si>
+  <si>
+    <t>Como gerente, quiero tener conocimiento si la campaña necesita matenimiento.</t>
+  </si>
+  <si>
+    <t>Como gerente, quiero tener conocimiento el rendimiento de la campaña.</t>
+  </si>
+  <si>
+    <t>Como acesor, necesito conocer el resultado de la campaña.</t>
+  </si>
+  <si>
+    <t>Mantenimiento.</t>
+  </si>
+  <si>
+    <t>Mantenimiento de tecnologias y marketing.</t>
+  </si>
+  <si>
+    <t>HU-019</t>
+  </si>
+  <si>
+    <t>HU-020</t>
+  </si>
+  <si>
+    <t>Documentación.</t>
+  </si>
+  <si>
+    <t>Como gerente, quiero hacer un analisis si la campaña es accesible para innovar.</t>
+  </si>
+  <si>
+    <t>Como gestor, necesito realizar la documentacion de resultados del la campaña.</t>
+  </si>
+  <si>
+    <t>Innovar.</t>
+  </si>
+  <si>
+    <t>Analisis de innovación.</t>
+  </si>
+  <si>
+    <t>Documentación de resultC21:I24ados.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,6 +420,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -433,9 +495,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -449,6 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I26"/>
+  <dimension ref="B1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +836,7 @@
   <sheetData>
     <row r="1" spans="2:9" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.35">
@@ -793,503 +853,566 @@
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="E5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="8">
+        <v>3</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="H5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="9">
-        <v>3</v>
-      </c>
-      <c r="G5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="8">
+        <v>2</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="9">
-        <v>2</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="E7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="8">
+        <v>2</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="H7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="9">
-        <v>2</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>32</v>
+      <c r="E8" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F8" s="7">
         <v>3</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>43</v>
+      <c r="G8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>32</v>
+      <c r="E9" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F9" s="7">
         <v>2</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>37</v>
+      <c r="G9" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>51</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" s="7">
         <v>5</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="E11" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F11" s="7">
         <v>8</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>61</v>
-      </c>
       <c r="E12" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F12" s="7">
         <v>5</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="E13" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F13" s="7">
         <v>5</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>69</v>
-      </c>
       <c r="E14" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F14" s="7">
         <v>8</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>73</v>
-      </c>
       <c r="E15" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F15" s="7">
         <v>3</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>77</v>
-      </c>
       <c r="E16" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F16" s="7">
         <v>8</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="E17" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F17" s="7">
         <v>2</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>85</v>
-      </c>
       <c r="E18" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F18" s="7">
         <v>13</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>89</v>
-      </c>
       <c r="E19" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F19" s="7">
         <v>5</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I19" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="7">
+        <v>9</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="8" t="s">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="7">
+        <v>9</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="7">
         <v>8</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="G22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="7">
         <v>8</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="G23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
+      <c r="B24" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="7">
+        <v>10</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1317,12 +1440,12 @@
   <sheetData>
     <row r="1" spans="2:3" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -1338,7 +1461,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="90" x14ac:dyDescent="0.25">
@@ -1346,55 +1469,55 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="225" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1404,11 +1527,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2622ba91-40fd-4640-b50c-92dc66e1fc44" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1639,27 +1763,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2622ba91-40fd-4640-b50c-92dc66e1fc44" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33A64BD6-8F16-4544-8B5D-AA544397FAEB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DA4B32A-075A-41C6-B17C-09D553423F42}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2622ba91-40fd-4640-b50c-92dc66e1fc44"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="749d5ae2-5db7-4e69-a7a3-6fccc2fcb882"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1684,9 +1798,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DA4B32A-075A-41C6-B17C-09D553423F42}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33A64BD6-8F16-4544-8B5D-AA544397FAEB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2622ba91-40fd-4640-b50c-92dc66e1fc44"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="749d5ae2-5db7-4e69-a7a3-6fccc2fcb882"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>